<commit_message>
Moving the data to the right file
</commit_message>
<xml_diff>
--- a/data/fd38_qPCR.xlsx
+++ b/data/fd38_qPCR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96853263-3931-B244-9460-E82D3C34477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B231DA-6B01-7E4B-96E6-A4372B4526F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{9D9DA09B-D1CF-084E-BE2E-E560D9A78A54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9D9DA09B-D1CF-084E-BE2E-E560D9A78A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>A1</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>C3</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
   <si>
     <t>D2</t>
@@ -436,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F3CC-AE5E-E440-8649-34660A564AA4}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -478,8 +481,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -511,10 +517,13 @@
         <v>32.029964157646297</v>
       </c>
       <c r="K2" s="1">
+        <v>34.426564717522503</v>
+      </c>
+      <c r="L2" s="1">
         <v>32.272718109441101</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,10 +553,13 @@
         <v>32.541351638432602</v>
       </c>
       <c r="K3" s="1">
+        <v>35.173269496183302</v>
+      </c>
+      <c r="L3" s="1">
         <v>32.354724267277099</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -575,6 +587,9 @@
         <v>32.606522462184003</v>
       </c>
       <c r="K4" s="1">
+        <v>35.4959667909053</v>
+      </c>
+      <c r="L4" s="1">
         <v>32.752593145860203</v>
       </c>
     </row>

</xml_diff>